<commit_message>
Added a parts manual
</commit_message>
<xml_diff>
--- a/ABS Valve Test BOM.xlsx
+++ b/ABS Valve Test BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="132">
   <si>
     <t>120VAC to 24VDC Transformer</t>
   </si>
@@ -397,6 +397,21 @@
   </si>
   <si>
     <t>300-S18N30F10</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Received?</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>n-partial (3/20)</t>
   </si>
 </sst>
 </file>
@@ -847,7 +862,7 @@
   <dimension ref="A7:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +871,8 @@
     <col min="2" max="2" width="47.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="4" customWidth="1"/>
-    <col min="5" max="10" width="9.140625" style="4"/>
+    <col min="5" max="9" width="9.140625" style="4"/>
+    <col min="10" max="10" width="20.42578125" style="4" customWidth="1"/>
     <col min="11" max="11" width="23.140625" style="4" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -889,6 +905,9 @@
       <c r="I7" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="J7" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -913,7 +932,12 @@
       <c r="H8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -938,7 +962,12 @@
       <c r="H9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -963,7 +992,12 @@
       <c r="H10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -988,7 +1022,12 @@
       <c r="H11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -1013,7 +1052,12 @@
       <c r="H12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
@@ -1038,7 +1082,12 @@
       <c r="H13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1063,7 +1112,12 @@
       <c r="H14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="8"/>
+      <c r="I14" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
@@ -1080,6 +1134,12 @@
       </c>
       <c r="H15" s="4" t="s">
         <v>6</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>55</v>
@@ -1112,9 +1172,14 @@
       <c r="H16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>17</v>
       </c>
@@ -1136,9 +1201,14 @@
       <c r="H17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>18</v>
@@ -1161,9 +1231,14 @@
       <c r="H18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
@@ -1185,9 +1260,14 @@
       <c r="H19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>21</v>
@@ -1210,9 +1290,14 @@
       <c r="H20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>22</v>
       </c>
@@ -1235,9 +1320,14 @@
       <c r="H21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>26</v>
@@ -1261,9 +1351,14 @@
       <c r="H22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>29</v>
       </c>
@@ -1286,9 +1381,14 @@
       <c r="H23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>36</v>
@@ -1312,9 +1412,14 @@
       <c r="H24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>38</v>
       </c>
@@ -1337,9 +1442,14 @@
       <c r="H25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>40</v>
@@ -1363,9 +1473,14 @@
       <c r="H26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>44</v>
       </c>
@@ -1388,9 +1503,14 @@
       <c r="H27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>47</v>
@@ -1414,9 +1534,14 @@
       <c r="H28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>49</v>
       </c>
@@ -1439,9 +1564,14 @@
       <c r="H29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>51</v>
@@ -1465,9 +1595,14 @@
       <c r="H30" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>56</v>
       </c>
@@ -1489,8 +1624,14 @@
       <c r="H31" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
         <v>58</v>
@@ -1513,9 +1654,22 @@
       <c r="H32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>62</v>
@@ -1540,10 +1694,13 @@
         <v>19</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>64</v>
       </c>
@@ -1569,8 +1726,11 @@
       <c r="I35" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>66</v>
@@ -1593,9 +1753,14 @@
       <c r="H36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I36" s="8"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>68</v>
       </c>
@@ -1617,9 +1782,14 @@
       <c r="H37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I37" s="6"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>69</v>
@@ -1632,9 +1802,14 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>70</v>
       </c>
@@ -1656,9 +1831,14 @@
       <c r="H39" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="6"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
         <v>72</v>
@@ -1681,9 +1861,14 @@
       <c r="H40" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="8"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>76</v>
       </c>
@@ -1708,8 +1893,11 @@
       <c r="I41" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>78</v>
@@ -1735,8 +1923,11 @@
       <c r="I42" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>80</v>
       </c>
@@ -1761,8 +1952,11 @@
       <c r="I43" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>82</v>
@@ -1788,8 +1982,11 @@
       <c r="I44" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
         <v>84</v>
       </c>
@@ -1814,8 +2011,11 @@
       <c r="I45" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
         <v>86</v>
@@ -1841,8 +2041,11 @@
       <c r="I46" s="8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>88</v>
       </c>
@@ -1867,8 +2070,11 @@
       <c r="I47" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
         <v>89</v>
@@ -1893,6 +2099,9 @@
       </c>
       <c r="I48" s="8" t="s">
         <v>125</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +2141,7 @@
     <hyperlink ref="H48" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId34"/>
+  <pageSetup scale="61" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId34"/>
 </worksheet>
 </file>
 
@@ -1944,7 +2153,7 @@
   <dimension ref="A7:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +2163,8 @@
     <col min="3" max="3" width="17.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="11" customWidth="1"/>
     <col min="5" max="8" width="9.140625" style="11" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="11"/>
+    <col min="9" max="9" width="9.140625" style="11"/>
+    <col min="10" max="10" width="18.5703125" style="11" customWidth="1"/>
     <col min="11" max="11" width="21" style="11" customWidth="1"/>
     <col min="12" max="12" width="16.5703125" style="11" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="11"/>
@@ -1985,6 +2195,12 @@
       <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -2010,6 +2226,12 @@
       <c r="H8" s="14" t="s">
         <v>19</v>
       </c>
+      <c r="I8" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
@@ -2033,6 +2255,12 @@
       </c>
       <c r="H9" s="12" t="s">
         <v>19</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2059,6 +2287,12 @@
       <c r="H10" s="14" t="s">
         <v>19</v>
       </c>
+      <c r="I10" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="K10" s="11" t="s">
         <v>99</v>
       </c>
@@ -2089,6 +2323,12 @@
       </c>
       <c r="H11" s="12" t="s">
         <v>19</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2115,6 +2355,12 @@
       <c r="H12" s="14" t="s">
         <v>19</v>
       </c>
+      <c r="I12" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
@@ -2138,6 +2384,12 @@
       </c>
       <c r="H13" s="12" t="s">
         <v>19</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2164,6 +2416,12 @@
       <c r="H14" s="14" t="s">
         <v>19</v>
       </c>
+      <c r="I14" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="N14" s="11" t="s">
         <v>112</v>
       </c>
@@ -2191,6 +2449,12 @@
       <c r="H15" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="I15" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
@@ -2212,6 +2476,12 @@
         <f t="shared" si="0"/>
         <v>230.4</v>
       </c>
+      <c r="I16" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="N16" s="11" t="s">
         <v>113</v>
       </c>
@@ -2239,6 +2509,12 @@
         <f>E17*F17</f>
         <v>930.15</v>
       </c>
+      <c r="I17" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>130</v>
+      </c>
       <c r="N17" s="11">
         <v>67</v>
       </c>
@@ -2273,6 +2549,12 @@
         <f>E18*F18</f>
         <v>201.92</v>
       </c>
+      <c r="I18" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="N18" s="11">
         <v>40</v>
       </c>
@@ -2307,6 +2589,12 @@
         <f>E19*F19</f>
         <v>289.8</v>
       </c>
+      <c r="I19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>131</v>
+      </c>
       <c r="N19" s="11">
         <v>48.5</v>
       </c>
@@ -2340,6 +2628,12 @@
       <c r="G20" s="11">
         <f>E20*F20</f>
         <v>223.72</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="P20" s="11">
         <f>SUM(P17:P19)</f>

</xml_diff>